<commit_message>
CE 6 and CE 7 knitted
</commit_message>
<xml_diff>
--- a/Data/Uppgiftsdata.xlsx
+++ b/Data/Uppgiftsdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="X:\Grundläggande statistik med tillämpningar inom naturvetenskap\R\R-anvisningar\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\storage-al.slu.se\home$\adfl0001\My Documents\Eget\Kurser (lärare)\Grundläggande statistik med tillämpningar inom naturvetenskap HT22\R-anvisningar\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A554A60-CC13-408B-8A4E-43956493F009}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70D295AE-33F1-4D36-841F-1ADC18729DC4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="928" firstSheet="1" activeTab="7" xr2:uid="{E21B11A5-3983-4CC8-B401-B14B36A292D4}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" tabRatio="928" firstSheet="3" activeTab="20" xr2:uid="{E21B11A5-3983-4CC8-B401-B14B36A292D4}"/>
   </bookViews>
   <sheets>
     <sheet name="Frilandskrysantemum" sheetId="1" r:id="rId1"/>
@@ -33,6 +33,7 @@
     <sheet name="Morötter" sheetId="17" r:id="rId18"/>
     <sheet name="Metodjämförelse" sheetId="18" r:id="rId19"/>
     <sheet name="Darwin" sheetId="19" r:id="rId20"/>
+    <sheet name="Bakterier" sheetId="21" r:id="rId21"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -53,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="278" uniqueCount="73">
   <si>
     <t>Planthöjd</t>
   </si>
@@ -130,9 +131,6 @@
     <t>Ekologisk</t>
   </si>
   <si>
-    <t>Behandling</t>
-  </si>
-  <si>
     <t>a1b1</t>
   </si>
   <si>
@@ -251,6 +249,30 @@
   </si>
   <si>
     <t>Vikt</t>
+  </si>
+  <si>
+    <t>Färg</t>
+  </si>
+  <si>
+    <t>Block</t>
+  </si>
+  <si>
+    <t>Cultivar</t>
+  </si>
+  <si>
+    <t>Inoculation</t>
+  </si>
+  <si>
+    <t>Dry weight</t>
+  </si>
+  <si>
+    <t>Control</t>
+  </si>
+  <si>
+    <t>Dead</t>
+  </si>
+  <si>
+    <t>Living</t>
   </si>
 </sst>
 </file>
@@ -813,25 +835,27 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4BFA08BC-3332-4743-BA80-14CCEF3F7614}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" t="s">
         <v>25</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>26</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>27</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>28</v>
-      </c>
-      <c r="E1" t="s">
-        <v>29</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
@@ -917,10 +941,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
         <v>30</v>
-      </c>
-      <c r="B1" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1165,7 +1189,7 @@
         <v>16</v>
       </c>
       <c r="B1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1279,15 +1303,15 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B2">
         <v>24</v>
@@ -1295,7 +1319,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B3">
         <v>18</v>
@@ -1303,7 +1327,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B4">
         <v>18</v>
@@ -1311,7 +1335,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B5">
         <v>29</v>
@@ -1319,7 +1343,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B6">
         <v>22</v>
@@ -1327,7 +1351,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B7">
         <v>17</v>
@@ -1335,7 +1359,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B8">
         <v>15</v>
@@ -1343,7 +1367,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B9">
         <v>46</v>
@@ -1351,7 +1375,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B10">
         <v>39</v>
@@ -1359,7 +1383,7 @@
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B11">
         <v>37</v>
@@ -1367,7 +1391,7 @@
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B12">
         <v>50</v>
@@ -1375,7 +1399,7 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B13">
         <v>44</v>
@@ -1383,7 +1407,7 @@
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B14">
         <v>45</v>
@@ -1391,7 +1415,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B15">
         <v>30</v>
@@ -1399,7 +1423,7 @@
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B16">
         <v>32</v>
@@ -1407,7 +1431,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B17">
         <v>30</v>
@@ -1415,7 +1439,7 @@
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B18">
         <v>26</v>
@@ -1423,7 +1447,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B19">
         <v>41</v>
@@ -1431,7 +1455,7 @@
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B20">
         <v>36</v>
@@ -1439,7 +1463,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B21">
         <v>28</v>
@@ -1447,7 +1471,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B22">
         <v>27</v>
@@ -1468,21 +1492,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>37</v>
+      </c>
+      <c r="B1" t="s">
         <v>38</v>
       </c>
-      <c r="B1" t="s">
-        <v>39</v>
-      </c>
       <c r="C1" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C2">
         <v>62</v>
@@ -1490,10 +1514,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>64</v>
@@ -1501,10 +1525,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C4">
         <v>64</v>
@@ -1512,10 +1536,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C5">
         <v>65</v>
@@ -1523,10 +1547,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C6">
         <v>66</v>
@@ -1534,10 +1558,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C7">
         <v>63</v>
@@ -1545,10 +1569,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C8">
         <v>63</v>
@@ -1556,10 +1580,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B9" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C9">
         <v>66</v>
@@ -1567,10 +1591,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B10" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C10">
         <v>67</v>
@@ -1578,10 +1602,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C11">
         <v>64</v>
@@ -1589,10 +1613,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C12">
         <v>61</v>
@@ -1600,10 +1624,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C13">
         <v>64</v>
@@ -1611,10 +1635,10 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C14">
         <v>65</v>
@@ -1622,10 +1646,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C15">
         <v>62</v>
@@ -1633,10 +1657,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C16">
         <v>65</v>
@@ -1644,10 +1668,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" t="s">
         <v>43</v>
-      </c>
-      <c r="B17" t="s">
-        <v>44</v>
       </c>
       <c r="C17">
         <v>55</v>
@@ -1655,10 +1679,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B18" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C18">
         <v>56</v>
@@ -1666,10 +1690,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B19" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C19">
         <v>60</v>
@@ -1677,10 +1701,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B20" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C20">
         <v>58</v>
@@ -1688,10 +1712,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B21" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C21">
         <v>59</v>
@@ -1712,13 +1736,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" t="s">
         <v>49</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>50</v>
-      </c>
-      <c r="C1" t="s">
-        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -1890,10 +1914,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>51</v>
+      </c>
+      <c r="B1" t="s">
         <v>52</v>
-      </c>
-      <c r="B1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -1991,13 +2015,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" t="s">
         <v>54</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>55</v>
-      </c>
-      <c r="C1" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2116,13 +2140,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" t="s">
         <v>57</v>
-      </c>
-      <c r="C1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2419,13 +2443,13 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
@@ -2433,7 +2457,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C2" s="1">
         <v>17.399999999999999</v>
@@ -2444,7 +2468,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C3" s="1">
         <v>20.399999999999999</v>
@@ -2455,7 +2479,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C4" s="1">
         <v>20</v>
@@ -2466,7 +2490,7 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C5" s="1">
         <v>20</v>
@@ -2477,7 +2501,7 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C6" s="1">
         <v>18.399999999999999</v>
@@ -2488,7 +2512,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C7" s="1">
         <v>18.600000000000001</v>
@@ -2499,7 +2523,7 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C8" s="1">
         <v>18.600000000000001</v>
@@ -2510,7 +2534,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C9" s="1">
         <v>15.3</v>
@@ -2521,7 +2545,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C10" s="1">
         <v>16.5</v>
@@ -2532,7 +2556,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1">
         <v>18</v>
@@ -2543,7 +2567,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C12" s="1">
         <v>16.3</v>
@@ -2554,7 +2578,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C13" s="1">
         <v>18</v>
@@ -2565,7 +2589,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C14" s="1">
         <v>12.8</v>
@@ -2576,7 +2600,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C15" s="1">
         <v>15.5</v>
@@ -2587,7 +2611,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C16" s="1">
         <v>18</v>
@@ -2598,7 +2622,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C17" s="1">
         <v>23.5</v>
@@ -2609,7 +2633,7 @@
         <v>17</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C18" s="1">
         <v>12</v>
@@ -2620,7 +2644,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C19" s="1">
         <v>21</v>
@@ -2631,7 +2655,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C20" s="1">
         <v>22</v>
@@ -2642,7 +2666,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C21" s="1">
         <v>19.100000000000001</v>
@@ -2653,7 +2677,7 @@
         <v>21</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C22" s="1">
         <v>21.5</v>
@@ -2664,7 +2688,7 @@
         <v>22</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C23" s="1">
         <v>22.1</v>
@@ -2675,7 +2699,7 @@
         <v>23</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C24" s="1">
         <v>20.399999999999999</v>
@@ -2686,7 +2710,7 @@
         <v>24</v>
       </c>
       <c r="B25" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C25" s="1">
         <v>18.3</v>
@@ -2697,7 +2721,7 @@
         <v>25</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C26" s="1">
         <v>21.6</v>
@@ -2708,7 +2732,7 @@
         <v>26</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C27" s="1">
         <v>23.3</v>
@@ -2719,7 +2743,7 @@
         <v>27</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C28" s="1">
         <v>21</v>
@@ -2730,7 +2754,7 @@
         <v>28</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C29" s="1">
         <v>22.1</v>
@@ -2741,7 +2765,7 @@
         <v>29</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C30" s="1">
         <v>23</v>
@@ -2752,10 +2776,373 @@
         <v>30</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C31" s="1">
         <v>12</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70E06FF7-6D25-4DEC-8D12-9049700FF39F}">
+  <dimension ref="A1:D25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D2" s="1">
+        <v>27.4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D3" s="1">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="1">
+        <v>1</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" s="1">
+        <v>34.5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="1">
+        <v>1</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D5" s="1">
+        <v>29.4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D6" s="1">
+        <v>32.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>1</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D7" s="1">
+        <v>34.4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1">
+        <v>2</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D8" s="1">
+        <v>28.9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="1">
+        <v>2</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D9" s="1">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1">
+        <v>2</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D10" s="1">
+        <v>33.4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="1">
+        <v>2</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D11" s="1">
+        <v>28.7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="1">
+        <v>2</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D12" s="1">
+        <v>32.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>2</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="1">
+        <v>36.4</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="1">
+        <v>3</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D14" s="1">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="1">
+        <v>3</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D15" s="1">
+        <v>29.7</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="1">
+        <v>3</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="1">
+        <v>32.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="1">
+        <v>3</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D17" s="1">
+        <v>27.2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="1">
+        <v>3</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D18" s="1">
+        <v>29.1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" s="1">
+        <v>3</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D19" s="1">
+        <v>32.6</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A20" s="1">
+        <v>4</v>
+      </c>
+      <c r="B20" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D20" s="1">
+        <v>26.7</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="1">
+        <v>4</v>
+      </c>
+      <c r="B21" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="1">
+        <v>28.9</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="1">
+        <v>4</v>
+      </c>
+      <c r="B22" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D22" s="1">
+        <v>31.8</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="1">
+        <v>4</v>
+      </c>
+      <c r="B23" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="D23" s="1">
+        <v>26.8</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A24" s="1">
+        <v>4</v>
+      </c>
+      <c r="B24" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="1">
+        <v>28.6</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="1">
+        <v>4</v>
+      </c>
+      <c r="B25" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D25" s="1">
+        <v>30.7</v>
       </c>
     </row>
   </sheetData>
@@ -3097,16 +3484,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5741B50E-3483-4D77-87BF-3956FCFEA119}">
   <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B1" t="s">
         <v>64</v>
-      </c>
-      <c r="B1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>